<commit_message>
update files and add todo's
</commit_message>
<xml_diff>
--- a/deployer dev stack/deployer stack resource spread across prox1 and prox2.xlsx
+++ b/deployer dev stack/deployer stack resource spread across prox1 and prox2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhys\Documents\Go\R710\ons-deployer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhys\Documents\Go\R710\gitgub-files\R710\deployer dev stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -224,10 +224,10 @@
     <t>on Proxmox Hypervisor to test and develop deployer</t>
   </si>
   <si>
-    <t>NOTE: Management box - install Desktop Ubuntu GUI + go + vscode to debug deployer</t>
-  </si>
-  <si>
     <t>Distribution of Ubuntu 20.04 LTS Server VM's across prox1 and prox2</t>
+  </si>
+  <si>
+    <t>NOTE: Management box - install Desktop Ubuntu GUI (minimal install) + go + vscode to debug deployer</t>
   </si>
 </sst>
 </file>
@@ -259,12 +259,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -279,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -293,6 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +583,7 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +596,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
@@ -680,7 +687,7 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L8">
         <v>930</v>
@@ -693,7 +700,7 @@
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <v>6</v>
       </c>
       <c r="E9">
@@ -710,16 +717,16 @@
         <f>H8-G9</f>
         <v>18</v>
       </c>
+      <c r="I9">
+        <v>40</v>
+      </c>
       <c r="J9">
         <f>J8-I9</f>
-        <v>176</v>
-      </c>
-      <c r="K9">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L15" si="1">L8-K9</f>
-        <v>780</v>
+        <v>930</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -729,7 +736,7 @@
       <c r="C10" s="5">
         <v>203</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <v>5</v>
       </c>
       <c r="E10">
@@ -747,15 +754,15 @@
         <v>16</v>
       </c>
       <c r="I10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J10">
         <f>J9-I10</f>
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>780</v>
+        <v>930</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -783,15 +790,15 @@
         <v>14</v>
       </c>
       <c r="I11">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J11">
         <f>J10-I11</f>
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>780</v>
+        <v>930</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -819,15 +826,15 @@
         <v>12</v>
       </c>
       <c r="I12">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J12">
         <f t="shared" ref="J12:J15" si="3">J11-I12</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
-        <v>780</v>
+        <v>930</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -856,14 +863,14 @@
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K13">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
-        <v>630</v>
+        <v>730</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -892,14 +899,14 @@
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K14">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -928,10 +935,10 @@
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K15">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
@@ -946,7 +953,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1031,7 +1038,7 @@
         <v>22</v>
       </c>
       <c r="J23">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L23">
         <v>930</v>
@@ -1063,7 +1070,7 @@
       </c>
       <c r="J24">
         <f>J23-I24</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K24">
         <v>100</v>
@@ -1099,7 +1106,7 @@
       </c>
       <c r="J25">
         <f>J24-I25</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K25">
         <v>100</v>
@@ -1135,7 +1142,7 @@
       </c>
       <c r="J26">
         <f>J25-I26</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K26">
         <v>100</v>
@@ -1171,7 +1178,7 @@
       </c>
       <c r="J27">
         <f t="shared" ref="J27:J30" si="7">J26-I27</f>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K27">
         <v>100</v>
@@ -1207,7 +1214,7 @@
       </c>
       <c r="J28">
         <f t="shared" si="7"/>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K28">
         <v>100</v>
@@ -1243,7 +1250,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="7"/>
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K29">
         <v>100</v>
@@ -1282,7 +1289,7 @@
       </c>
       <c r="J30">
         <f t="shared" si="7"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L30">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
Add deployer estate plan
</commit_message>
<xml_diff>
--- a/deployer dev stack/deployer stack resource spread across prox1 and prox2.xlsx
+++ b/deployer dev stack/deployer stack resource spread across prox1 and prox2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>RAM</t>
   </si>
@@ -170,9 +170,6 @@
     <t>mongo</t>
   </si>
   <si>
-    <t>Management box - deployer, bastion (?)</t>
-  </si>
-  <si>
     <t>man</t>
   </si>
   <si>
@@ -228,6 +225,42 @@
   </si>
   <si>
     <t>NOTE: Management box - install Desktop Ubuntu GUI (minimal install) + go + vscode to debug deployer</t>
+  </si>
+  <si>
+    <t>Setup Rpi with SSD as a fileserver</t>
+  </si>
+  <si>
+    <t>Ansible</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>Terraform stack order setup:</t>
+  </si>
+  <si>
+    <t>See the readme file in dp-setup/terraform</t>
+  </si>
+  <si>
+    <t>add 100G of Raid 1 to management box and run up file server, etc ?</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>deployer, bastion (?)</t>
+  </si>
+  <si>
+    <t>dep</t>
+  </si>
+  <si>
+    <t>NOTE: Servers on prox2 have neptune client installed</t>
   </si>
 </sst>
 </file>
@@ -259,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +302,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -300,6 +345,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,32 +641,32 @@
     <col min="11" max="11" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -628,10 +675,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>0</v>
       </c>
@@ -653,18 +703,24 @@
       <c r="L6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>11</v>
@@ -693,9 +749,9 @@
         <v>930</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>13</v>
@@ -707,8 +763,8 @@
         <f t="shared" ref="E9:E15" si="0">E8-D9</f>
         <v>36</v>
       </c>
-      <c r="F9" t="s">
-        <v>49</v>
+      <c r="F9" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="G9" s="3">
         <v>4</v>
@@ -724,12 +780,24 @@
         <f>J8-I9</f>
         <v>134</v>
       </c>
+      <c r="K9" s="9">
+        <v>100</v>
+      </c>
       <c r="L9">
-        <f t="shared" ref="L9:L15" si="1">L8-K9</f>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <f>L8-K9</f>
+        <v>830</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -750,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H15" si="2">H9-G10</f>
+        <f t="shared" ref="H10:H15" si="1">H9-G10</f>
         <v>16</v>
       </c>
       <c r="I10">
@@ -761,18 +829,18 @@
         <v>94</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="L10:L15" si="2">L9-K10</f>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="5">
         <v>204</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>5</v>
       </c>
       <c r="E11">
@@ -786,7 +854,7 @@
         <v>2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="I11">
@@ -797,18 +865,18 @@
         <v>54</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="5">
         <v>205</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="7">
         <v>4</v>
       </c>
       <c r="E12">
@@ -822,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I12">
@@ -833,18 +901,18 @@
         <v>24</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
-        <v>930</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="5">
         <v>206</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="7">
         <v>7</v>
       </c>
       <c r="E13">
@@ -852,13 +920,13 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13">
         <v>4</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J13">
@@ -869,18 +937,18 @@
         <v>200</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
-        <v>730</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="5">
         <v>207</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="7">
         <v>7</v>
       </c>
       <c r="E14">
@@ -888,13 +956,13 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14">
         <v>4</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J14">
@@ -905,18 +973,18 @@
         <v>200</v>
       </c>
       <c r="L14">
-        <f t="shared" si="1"/>
-        <v>530</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="6">
         <v>208</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>7</v>
       </c>
       <c r="E15">
@@ -924,13 +992,13 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15">
         <v>4</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J15">
@@ -941,11 +1009,11 @@
         <v>200</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
         <v>14</v>
       </c>
@@ -953,7 +1021,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -963,14 +1031,14 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -979,10 +1047,14 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="4"/>
       <c r="D21" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1079,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>8</v>
@@ -1015,7 +1087,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>7</v>
@@ -1051,11 +1123,11 @@
       <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <v>5</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E30" si="4">E23-D24</f>
+        <f t="shared" ref="E24:E31" si="4">E23-D24</f>
         <v>37</v>
       </c>
       <c r="F24" t="s">
@@ -1076,7 +1148,7 @@
         <v>100</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L30" si="5">L23-K24</f>
+        <f t="shared" ref="L24:L31" si="5">L23-K24</f>
         <v>830</v>
       </c>
     </row>
@@ -1087,7 +1159,7 @@
       <c r="C25" s="5">
         <v>223</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="7">
         <v>5</v>
       </c>
       <c r="E25">
@@ -1101,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H30" si="6">H24-G25</f>
+        <f t="shared" ref="H25:H31" si="6">H24-G25</f>
         <v>18</v>
       </c>
       <c r="J25">
@@ -1123,22 +1195,22 @@
       <c r="C26" s="5">
         <v>224</v>
       </c>
-      <c r="D26">
-        <v>8</v>
+      <c r="D26" s="9">
+        <v>7</v>
       </c>
       <c r="E26">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="3">
-        <v>5</v>
+        <v>49</v>
+      </c>
+      <c r="G26" s="9">
+        <v>4</v>
       </c>
       <c r="H26">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J26">
         <f>J25-I26</f>
@@ -1151,6 +1223,9 @@
         <f t="shared" si="5"/>
         <v>630</v>
       </c>
+      <c r="N26" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
@@ -1159,25 +1234,25 @@
       <c r="C27" s="5">
         <v>225</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <v>5</v>
       </c>
       <c r="E27">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
       <c r="H27">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27:J30" si="7">J26-I27</f>
+        <f t="shared" ref="J27:J31" si="7">J26-I27</f>
         <v>174</v>
       </c>
       <c r="K27">
@@ -1195,22 +1270,22 @@
       <c r="C28" s="5">
         <v>226</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>5</v>
       </c>
       <c r="E28">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="H28">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J28">
         <f t="shared" si="7"/>
@@ -1231,22 +1306,22 @@
       <c r="C29" s="5">
         <v>227</v>
       </c>
-      <c r="D29">
-        <v>8</v>
+      <c r="D29" s="9">
+        <v>7</v>
       </c>
       <c r="E29">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29">
-        <v>5</v>
+        <v>50</v>
+      </c>
+      <c r="G29" s="9">
+        <v>4</v>
       </c>
       <c r="H29">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J29">
         <f t="shared" si="7"/>
@@ -1267,12 +1342,12 @@
       <c r="C30" s="6">
         <v>228</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="7">
         <v>6</v>
       </c>
       <c r="E30">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
         <v>47</v>
@@ -1282,14 +1357,14 @@
       </c>
       <c r="H30">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="J30">
         <f t="shared" si="7"/>
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="L30">
         <f t="shared" si="5"/>
@@ -1297,104 +1372,156 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I31" t="s">
-        <v>14</v>
-      </c>
-      <c r="O31" s="2"/>
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="6">
+        <v>229</v>
+      </c>
+      <c r="D31" s="9">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="9">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>20</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="7"/>
+        <v>54</v>
+      </c>
+      <c r="L31">
+        <f>L30-K31</f>
+        <v>330</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I32" t="s">
+        <v>14</v>
+      </c>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="8"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>54</v>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>